<commit_message>
Tue Jan 11 01:34:55 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -233,7 +233,7 @@
 作业</t>
   </si>
   <si>
-    <t>肩</t>
+    <t>背</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1300,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -1508,8 +1508,8 @@
       <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
+      <c r="E13" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>7</v>
@@ -1527,15 +1527,13 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="H14" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A16" s="2"/>

</xml_diff>

<commit_message>
Wed Feb 16 17:53:59 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780" activeTab="3"/>
+    <workbookView windowWidth="21600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="02" sheetId="3" r:id="rId3"/>
     <sheet name="03" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
   <si>
     <t>早餐</t>
   </si>
@@ -262,6 +262,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>10技术书</t>
@@ -677,48 +678,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
 1音频/视频
 </t>
     </r>
@@ -832,6 +791,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -928,12 +894,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1003,12 +977,20 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1078,6 +1060,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -1289,6 +1278,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -1510,6 +1506,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1569,6 +1572,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -1596,6 +1605,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -1651,16 +1667,7 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
+      <t>10技术书</t>
     </r>
     <r>
       <rPr>
@@ -1677,30 +1684,21 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
@@ -1709,6 +1707,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -1720,7 +1719,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1759,13 +1758,28 @@
   </si>
   <si>
     <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1804,6 +1818,61 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -1821,10 +1890,134 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
 1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
 </sst>
@@ -1905,8 +2098,24 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1914,29 +2123,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1959,7 +2145,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1972,30 +2158,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2010,14 +2175,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2025,9 +2182,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2091,7 +2284,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2103,13 +2410,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2121,151 +2452,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2294,21 +2487,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2323,6 +2501,36 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2344,30 +2552,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2377,16 +2561,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2396,139 +2589,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3840,25 +4033,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="13" t="s">
+      <c r="G27" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>29</v>
-      </c>
       <c r="H27" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3876,7 +4069,7 @@
         <v>22</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3920,13 +4113,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3972,8 +4165,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4048,25 +4241,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4164,37 +4357,45 @@
         <v>3</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4261,7 +4462,7 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -4277,17 +4478,19 @@
         <v>41</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -4375,10 +4578,10 @@
         <v>42</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4428,8 +4631,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4510,19 +4713,19 @@
         <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">

</xml_diff>

<commit_message>
Thu Mar  3 00:24:20 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="02" sheetId="3" r:id="rId3"/>
     <sheet name="03" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>早餐</t>
   </si>
@@ -1667,13 +1667,30 @@
   </si>
   <si>
     <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1684,36 +1701,42 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
     </r>
     <r>
       <rPr>
@@ -1758,28 +1781,13 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1821,18 +1829,10 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
 </t>
     </r>
     <r>
@@ -1843,17 +1843,7 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
+      <t>20非技术书</t>
     </r>
     <r>
       <rPr>
@@ -1867,12 +1857,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
+    <t>跑步45分钟</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -1884,7 +1872,17 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20非技术书</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
     </r>
     <r>
       <rPr>
@@ -1994,8 +1992,40 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">10技术书
+    <t>跑步45分钟
+胸</t>
+  </si>
+  <si>
+    <t>跑步45分钟
+ 肩</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -2003,21 +2033,84 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
     </r>
   </si>
 </sst>
@@ -2026,9 +2119,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -2050,13 +2143,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2098,6 +2191,58 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -2106,7 +2251,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2121,38 +2266,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2168,23 +2283,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2204,35 +2303,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
       <charset val="134"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
@@ -2260,13 +2353,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.5"/>
+        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="6" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2284,7 +2377,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2296,7 +2461,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2308,157 +2551,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2483,6 +2576,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2535,6 +2643,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2552,35 +2671,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2589,139 +2682,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2734,7 +2827,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2750,13 +2843,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2768,10 +2867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2780,7 +2876,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2789,7 +2885,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3188,25 +3284,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3214,13 +3310,13 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3298,25 +3394,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3402,25 +3498,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3444,19 +3540,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="9">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="9">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="9">
         <v>28</v>
       </c>
     </row>
@@ -3500,25 +3596,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3536,13 +3632,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="9">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="9">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="9">
         <v>31</v>
       </c>
     </row>
@@ -3574,13 +3670,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3593,28 +3689,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3627,7 +3723,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -3695,10 +3791,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2"/>
@@ -3710,25 +3806,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3736,28 +3832,28 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2"/>
@@ -3826,25 +3922,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3854,14 +3950,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2"/>
@@ -3930,25 +4026,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3956,12 +4052,12 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2"/>
@@ -3976,19 +4072,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="9">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="9">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="9">
         <v>28</v>
       </c>
     </row>
@@ -4032,25 +4128,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4059,28 +4155,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="9">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="9">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="9">
         <v>31</v>
       </c>
     </row>
@@ -4112,13 +4208,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4131,28 +4227,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4165,8 +4261,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4240,25 +4336,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4266,28 +4362,28 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2"/>
@@ -4356,44 +4452,44 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>38</v>
+      <c r="H13" s="17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="2"/>
@@ -4462,25 +4558,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="F20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4488,7 +4584,7 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="2"/>
@@ -4506,19 +4602,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="9">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="9">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="9">
         <v>28</v>
       </c>
     </row>
@@ -4562,25 +4658,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="11" t="s">
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4591,34 +4687,42 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="E28" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="10"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="10"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="10"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4631,8 +4735,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4707,45 +4811,49 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="C5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>44</v>
+      <c r="H5" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -4816,25 +4924,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4920,25 +5028,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4962,19 +5070,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="9">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="9">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="9">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="9">
         <v>28</v>
       </c>
     </row>
@@ -5018,25 +5126,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5054,13 +5162,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="9">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="9">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="9">
         <v>31</v>
       </c>
     </row>
@@ -5092,13 +5200,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5111,28 +5219,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Mon Mar  7 14:32:13 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>早餐</t>
   </si>
@@ -1781,6 +1781,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1861,6 +1868,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2000,67 +2013,17 @@
  肩</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
+    <t>跑步45分钟
+ 腹</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2111,6 +2074,87 @@
       </rPr>
       <t xml:space="preserve">
 1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
 </sst>
@@ -2119,10 +2163,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2183,13 +2227,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -2198,10 +2235,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2220,38 +2281,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2266,16 +2304,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2290,7 +2328,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2303,11 +2341,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2371,25 +2415,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2401,13 +2433,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2419,37 +2457,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2467,7 +2481,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2479,79 +2595,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2604,11 +2648,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2628,21 +2693,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2650,21 +2700,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2677,147 +2712,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4261,8 +4305,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="D26" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4573,11 +4617,11 @@
       <c r="F20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>36</v>
+      <c r="G20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4735,8 +4779,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4854,10 +4898,16 @@
       <c r="C7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4925,22 +4975,22 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>6</v>
@@ -4952,16 +5002,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">

</xml_diff>

<commit_message>
Sun Mar 13 13:51:48 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
   <si>
     <t>早餐</t>
   </si>
@@ -1864,16 +1864,97 @@
     </r>
   </si>
   <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
     <t>跑步45分钟</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2017,67 +2098,17 @@
  腹</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
+    <t>跑步45分钟
+背</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2155,6 +2186,114 @@
       <t xml:space="preserve">
 1音频/视频
 作业</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
     </r>
   </si>
 </sst>
@@ -2163,9 +2302,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -2185,6 +2324,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -2202,7 +2348,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <strike/>
@@ -2210,18 +2355,124 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2236,51 +2487,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -2289,75 +2495,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2415,7 +2554,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2427,37 +2602,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2475,7 +2638,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2487,73 +2716,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2565,37 +2734,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2624,30 +2763,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2659,21 +2774,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2695,10 +2795,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2713,6 +2811,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2721,147 +2849,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2890,15 +3029,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2911,17 +3059,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2929,7 +3068,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3328,10 +3467,10 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -3343,10 +3482,10 @@
       <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3354,13 +3493,13 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3453,10 +3592,10 @@
       <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3551,16 +3690,16 @@
       <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3584,19 +3723,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="12">
         <v>24</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="12">
         <v>25</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="12">
         <v>26</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="12">
         <v>27</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="12">
         <v>28</v>
       </c>
     </row>
@@ -3640,25 +3779,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3676,13 +3815,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="9">
+      <c r="B30" s="12">
         <v>29</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="12">
         <v>30</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="12">
         <v>31</v>
       </c>
     </row>
@@ -3714,13 +3853,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3733,28 +3872,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="13"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="13"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="13"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3835,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="18" t="s">
@@ -3850,25 +3989,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3876,28 +4015,28 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2"/>
@@ -3966,25 +4105,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3994,14 +4133,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2"/>
@@ -4070,25 +4209,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4096,12 +4235,12 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2"/>
@@ -4116,19 +4255,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="12">
         <v>24</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="12">
         <v>25</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="12">
         <v>26</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="12">
         <v>27</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="12">
         <v>28</v>
       </c>
     </row>
@@ -4172,25 +4311,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4199,28 +4338,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="9">
+      <c r="B30" s="12">
         <v>29</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="12">
         <v>30</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="12">
         <v>31</v>
       </c>
     </row>
@@ -4252,13 +4391,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4271,28 +4410,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="13"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="13"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="13"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4305,8 +4444,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4380,25 +4519,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4406,28 +4545,28 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2"/>
@@ -4496,25 +4635,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4522,18 +4661,18 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="11" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="2"/>
@@ -4602,25 +4741,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4628,7 +4767,7 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="2"/>
@@ -4646,19 +4785,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="12">
         <v>24</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="12">
         <v>25</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="12">
         <v>26</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="12">
         <v>27</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="12">
         <v>28</v>
       </c>
     </row>
@@ -4702,25 +4841,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="D27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="F27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4731,42 +4870,42 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>42</v>
+      <c r="E28" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="13"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="13"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A34" s="11"/>
-      <c r="B34" s="10"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="13"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4779,8 +4918,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4855,24 +4994,24 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4880,35 +5019,37 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>42</v>
+      <c r="B7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="2"/>
+      <c r="F7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A9" s="2"/>
@@ -4974,37 +5115,45 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>48</v>
+      <c r="B13" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -5073,24 +5222,24 @@
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5114,19 +5263,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="12">
         <v>24</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="12">
         <v>25</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="12">
         <v>26</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="12">
         <v>27</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="12">
         <v>28</v>
       </c>
     </row>
@@ -5170,25 +5319,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5206,13 +5355,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="9">
+      <c r="B30" s="12">
         <v>29</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="12">
         <v>30</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="12">
         <v>31</v>
       </c>
     </row>
@@ -5244,13 +5393,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5263,28 +5412,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="13"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="13"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="13"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="11"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Sun Mar 20 20:59:46 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
     <sheet name="01" sheetId="1" r:id="rId2"/>
     <sheet name="02" sheetId="3" r:id="rId3"/>
     <sheet name="03" sheetId="4" r:id="rId4"/>
+    <sheet name="04" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
   <si>
     <t>早餐</t>
   </si>
@@ -552,6 +553,71 @@
   </si>
   <si>
     <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <strike/>
         <sz val="11"/>
@@ -1910,13 +1976,16 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1924,70 +1993,25 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
     <t>跑步45分钟</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2103,12 +2127,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2163,6 +2181,66 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2205,7 +2283,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2244,25 +2322,7 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">10技术书
 </t>
     </r>
     <r>
@@ -2273,23 +2333,12 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2324,10 +2373,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2337,9 +2385,10 @@
       <charset val="134"/>
     </font>
     <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2502,13 +2551,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
       <charset val="134"/>
     </font>
     <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
@@ -2536,13 +2585,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="6" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.5"/>
+        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3010,7 +3059,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3026,40 +3075,49 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3068,7 +3126,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3393,7 +3454,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="C10" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3467,25 +3528,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3493,13 +3554,13 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3577,25 +3638,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3681,25 +3742,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3723,19 +3784,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -3779,25 +3840,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3815,13 +3876,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="12">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="7">
         <v>31</v>
       </c>
     </row>
@@ -3853,13 +3914,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3872,28 +3933,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="15"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3906,8 +3967,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3974,10 +4035,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2"/>
@@ -3989,25 +4050,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4015,28 +4076,28 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2"/>
@@ -4105,26 +4166,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="D13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>25</v>
+      <c r="H13" s="15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4133,14 +4194,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2"/>
@@ -4209,25 +4270,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="B20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4235,12 +4296,12 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="18" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2"/>
@@ -4255,19 +4316,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -4311,26 +4372,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="5" t="s">
+      <c r="B27" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>28</v>
+      <c r="G27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4338,28 +4399,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>29</v>
+      <c r="H28" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="12">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="7">
         <v>31</v>
       </c>
     </row>
@@ -4391,14 +4452,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>30</v>
+      <c r="B34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4410,28 +4471,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="15"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4444,8 +4505,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4519,54 +4580,54 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="E5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="F5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>36</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="18" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2"/>
@@ -4635,25 +4696,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="B13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4661,18 +4722,18 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="2"/>
@@ -4741,25 +4802,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="D20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="F20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4767,8 +4828,8 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>29</v>
+      <c r="B21" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -4785,19 +4846,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -4841,26 +4902,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="D27" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>36</v>
+      <c r="E27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4870,42 +4931,42 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>44</v>
+      <c r="E28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="11"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4918,8 +4979,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4993,61 +5054,61 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>36</v>
+      <c r="G5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>44</v>
+      <c r="D7" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5115,47 +5176,51 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>52</v>
+      <c r="H13" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>44</v>
+      <c r="B14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A16" s="2"/>
@@ -5221,25 +5286,571 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>25</v>
+      </c>
+      <c r="F23" s="7">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
+        <v>30</v>
+      </c>
+      <c r="D30" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5263,19 +5874,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -5319,25 +5930,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5355,15 +5966,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="12">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="12">
-        <v>31</v>
-      </c>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -5371,7 +5980,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -5379,7 +5988,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A33" s="4" t="s">
@@ -5387,21 +5996,19 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
@@ -5409,31 +6016,31 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="15"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Tue Mar 22 00:21:19 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>早餐</t>
   </si>
@@ -1733,6 +1733,61 @@
   </si>
   <si>
     <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <strike/>
         <sz val="11"/>
@@ -2319,6 +2374,46 @@
       <t xml:space="preserve">
 1音频/视频</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <t>肩
+跑步45分钟</t>
   </si>
   <si>
     <r>
@@ -3967,7 +4062,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -4172,8 +4267,8 @@
       <c r="C13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>25</v>
+      <c r="D13" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>25</v>
@@ -4270,8 +4365,8 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>25</v>
+      <c r="B20" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>27</v>
@@ -4505,8 +4600,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4709,7 +4804,7 @@
         <v>38</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>20</v>
@@ -4806,16 +4901,16 @@
         <v>38</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>20</v>
@@ -4903,25 +4998,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="D27" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4932,16 +5027,16 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -4979,8 +5074,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5055,19 +5150,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>37</v>
@@ -5093,23 +5188,23 @@
         <v>8</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5180,22 +5275,22 @@
         <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>37</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5203,23 +5298,23 @@
         <v>8</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5287,19 +5382,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>55</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>6</v>
@@ -5313,23 +5408,21 @@
         <v>8</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5397,10 +5490,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>4</v>
@@ -5423,25 +5516,25 @@
         <v>8</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5485,7 +5578,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>4</v>
@@ -5499,13 +5592,13 @@
         <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">

</xml_diff>

<commit_message>
Sun Mar 27 14:40:58 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>早餐</t>
   </si>
@@ -705,6 +705,71 @@
   </si>
   <si>
     <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <strike/>
         <sz val="11"/>
@@ -897,14 +962,17 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
     </r>
     <r>
       <rPr>
@@ -944,7 +1012,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -992,10 +1079,30 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
     </r>
   </si>
   <si>
@@ -1047,6 +1154,109 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
+1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1083,14 +1293,17 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
     </r>
     <r>
       <rPr>
@@ -1130,7 +1343,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1166,13 +1398,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2179,6 +2404,61 @@
   </si>
   <si>
     <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -2395,6 +2675,31 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -3161,6 +3466,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3172,9 +3480,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4014,8 +4319,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4082,10 +4387,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2"/>
@@ -4097,19 +4402,19 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="20" t="s">
@@ -4136,15 +4441,15 @@
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2"/>
@@ -4213,19 +4518,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="12" t="s">
@@ -4241,14 +4546,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2"/>
@@ -4317,19 +4622,19 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="15" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="12" t="s">
@@ -4343,12 +4648,12 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2"/>
@@ -4419,26 +4724,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>28</v>
       </c>
+      <c r="C27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="G27" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4446,17 +4751,17 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="15" t="s">
-        <v>30</v>
+      <c r="H28" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4499,14 +4804,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>31</v>
+      <c r="B34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4553,7 +4858,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4627,26 +4932,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>33</v>
+      <c r="B5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4666,15 +4971,15 @@
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2"/>
@@ -4744,19 +5049,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>20</v>
@@ -4769,18 +5074,18 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="2"/>
@@ -4850,19 +5155,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>20</v>
@@ -4875,8 +5180,8 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>30</v>
+      <c r="B21" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -4950,19 +5255,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>20</v>
@@ -4978,17 +5283,17 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>43</v>
+      <c r="E28" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5026,8 +5331,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5102,25 +5407,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5140,23 +5445,23 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5224,49 +5529,49 @@
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>43</v>
+      <c r="B14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
-        <v>43</v>
+      <c r="F14" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5334,25 +5639,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5360,21 +5665,21 @@
         <v>8</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5442,13 +5747,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>4</v>
@@ -5469,20 +5774,18 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5526,7 +5829,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>4</v>
@@ -5540,13 +5843,13 @@
         <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5584,7 +5887,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mon Apr  4 13:00:25 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
   <si>
     <t>早餐</t>
   </si>
@@ -1354,6 +1354,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -1565,6 +1572,231 @@
         <charset val="134"/>
       </rPr>
       <t>页</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
   <si>
@@ -2273,16 +2505,11 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2295,6 +2522,61 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2439,11 +2721,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2461,38 +2738,10 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
 1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
     </r>
   </si>
 </sst>
@@ -2502,9 +2751,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2557,24 +2806,62 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2595,68 +2882,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -2664,15 +2889,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2687,7 +2906,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2753,7 +3002,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,43 +3158,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2813,127 +3176,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2962,11 +3211,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2986,17 +3274,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3015,197 +3308,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4646,8 +4895,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4730,17 +4979,17 @@
       <c r="D5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="15" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4838,19 +5087,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>20</v>
@@ -4944,19 +5193,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>20</v>
@@ -5044,19 +5293,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="D27" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>20</v>
@@ -5073,16 +5322,16 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5120,8 +5369,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5196,25 +5445,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5234,23 +5483,23 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5318,25 +5567,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>38</v>
+      <c r="D13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5344,23 +5593,23 @@
         <v>8</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5427,26 +5676,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="13" t="s">
         <v>51</v>
       </c>
+      <c r="C20" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="D20" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5454,21 +5703,21 @@
         <v>8</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5536,22 +5785,22 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>6</v>
@@ -5563,19 +5812,15 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
@@ -5617,8 +5862,8 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>43</v>
+      <c r="B34" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>4</v>
@@ -5631,14 +5876,12 @@
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>44</v>
+      <c r="B35" s="5"/>
+      <c r="C35" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5676,8 +5919,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5755,7 +5998,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Mon Apr  4 20:28:35 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
   <si>
     <t>早餐</t>
   </si>
@@ -1056,14 +1056,17 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
     </r>
     <r>
       <rPr>
@@ -1103,7 +1106,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1151,10 +1173,30 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
     </r>
   </si>
   <si>
@@ -1206,6 +1248,109 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
+1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1805,237 +1950,68 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿10页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+二次校对译稿10页
+二次校对译稿10页
 </t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -2046,62 +2022,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿10页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-二次校对译稿10页
-二次校对译稿10页
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
 </t>
     </r>
     <r>
@@ -2550,6 +2470,39 @@
         <charset val="134"/>
       </rPr>
       <t>视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
@@ -2724,53 +2677,80 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
     <t>肩
 跑步45分钟</t>
   </si>
   <si>
     <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -4443,8 +4423,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4931,11 +4911,11 @@
       <c r="B34" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>28</v>
+      <c r="C34" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4981,8 +4961,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5057,24 +5037,24 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5455,8 +5435,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5546,10 +5526,10 @@
         <v>47</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5569,10 +5549,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>46</v>
@@ -5582,10 +5562,10 @@
         <v>46</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5763,25 +5743,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="11" t="s">
         <v>55</v>
       </c>
+      <c r="F20" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="G20" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5886,10 +5866,10 @@
         <v>45</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5949,10 +5929,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>4</v>
@@ -6006,7 +5986,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6084,7 +6064,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Sun Apr 10 20:41:48 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
   <si>
     <t>早餐</t>
   </si>
@@ -777,117 +777,147 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
     </r>
   </si>
   <si>
@@ -1238,151 +1268,6 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
@@ -2492,39 +2377,6 @@
         <charset val="134"/>
       </rPr>
       <t>视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
     </r>
   </si>
   <si>
@@ -2696,6 +2548,39 @@
       </rPr>
       <t xml:space="preserve">
 1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
@@ -3219,13 +3104,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.5"/>
+        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="6" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3715,7 +3600,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3730,22 +3618,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3754,7 +3639,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4168,10 +4053,10 @@
       <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4184,8 +4069,8 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4278,10 +4163,10 @@
       <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4382,10 +4267,10 @@
       <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4409,19 +4294,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="8">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="8">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="8">
         <v>28</v>
       </c>
     </row>
@@ -4480,10 +4365,10 @@
       <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4501,13 +4386,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="8">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="8">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="8">
         <v>31</v>
       </c>
     </row>
@@ -4558,28 +4443,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4592,8 +4477,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4660,7 +4545,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -4706,23 +4591,23 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2"/>
@@ -4819,14 +4704,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2"/>
@@ -4921,12 +4806,12 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2"/>
@@ -4941,19 +4826,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="8">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="8">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="8">
         <v>28</v>
       </c>
     </row>
@@ -5000,23 +4885,23 @@
       <c r="B27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="18" t="s">
+      <c r="G27" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>30</v>
-      </c>
       <c r="H27" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5024,28 +4909,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>31</v>
+      <c r="H28" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="8">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="8">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="8">
         <v>31</v>
       </c>
     </row>
@@ -5078,13 +4963,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5096,28 +4981,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5130,7 +5015,7 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C21" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -5206,25 +5091,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="F5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="H5" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5236,23 +5121,23 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2"/>
@@ -5325,16 +5210,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>20</v>
@@ -5347,18 +5232,18 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="2"/>
@@ -5428,19 +5313,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>20</v>
@@ -5453,8 +5338,8 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>31</v>
+      <c r="B21" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5471,19 +5356,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="8">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="8">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="8">
         <v>28</v>
       </c>
     </row>
@@ -5528,19 +5413,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>20</v>
@@ -5556,42 +5441,42 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>46</v>
+      <c r="E28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="9"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="11"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5604,8 +5489,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5680,25 +5565,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5710,31 +5595,31 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5802,19 +5687,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>20</v>
@@ -5827,21 +5712,21 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>46</v>
+      <c r="B14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
-        <v>46</v>
+      <c r="F14" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -5910,25 +5795,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>48</v>
+      <c r="H20" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5936,21 +5821,21 @@
         <v>8</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5961,19 +5846,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="8">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="8">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="8">
         <v>28</v>
       </c>
     </row>
@@ -6018,25 +5903,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6045,7 +5930,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="15" t="s">
@@ -6057,13 +5942,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="8">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="8">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="8">
         <v>31</v>
       </c>
     </row>
@@ -6095,11 +5980,11 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>59</v>
+      <c r="B34" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>4</v>
@@ -6111,35 +5996,35 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -6152,8 +6037,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6228,25 +6113,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6258,8 +6143,8 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -6269,12 +6154,12 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="12" t="s">
-        <v>62</v>
+      <c r="H7" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6342,25 +6227,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>6</v>
+        <v>61</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6368,17 +6253,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6446,7 +6327,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>13</v>
@@ -6460,10 +6341,10 @@
       <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6487,19 +6368,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="8">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="8">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="8">
         <v>28</v>
       </c>
     </row>
@@ -6558,10 +6439,10 @@
       <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6579,13 +6460,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B30" s="8">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="8">
         <v>30</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -6593,7 +6474,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -6601,7 +6482,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="9"/>
+      <c r="D32" s="10"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A33" s="4" t="s">
@@ -6609,7 +6490,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="9"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
       <c r="A34" s="4" t="s">
@@ -6621,7 +6502,7 @@
       <c r="C34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="11"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
@@ -6629,31 +6510,31 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="9"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Thu Apr 14 21:49:39 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="1"/>
+    <workbookView windowHeight="16780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>早餐</t>
   </si>
@@ -712,71 +712,13 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -1123,45 +1065,22 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
     </r>
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
     </r>
     <r>
       <rPr>
@@ -1228,50 +1147,11 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页
+校对译稿10页</t>
     </r>
   </si>
   <si>
@@ -1283,7 +1163,17 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>10技术书</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
     </r>
     <r>
       <rPr>
@@ -1353,8 +1243,27 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>校对译稿10页
-校对译稿10页</t>
+      <t>二次校对译稿10页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿10页</t>
     </r>
   </si>
   <si>
@@ -1423,50 +1332,160 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿10页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿10页</t>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页</t>
     </r>
   </si>
   <si>
@@ -1690,241 +1709,85 @@
       </rPr>
       <t>页</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音频</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二次校对译稿10页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+二次校对译稿10页
+二次校对译稿10页
 </t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1956,77 +1819,76 @@
       </rPr>
       <t xml:space="preserve">
 1音频/视频
-作业
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>二次校对译稿10页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-二次校对译稿10页
-二次校对译稿10页
-</t>
+作业</t>
     </r>
   </si>
   <si>
     <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2043,7 +1905,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2089,23 +1951,13 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2148,7 +2000,7 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>10技术书</t>
@@ -2197,43 +2049,23 @@
   <si>
     <r>
       <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
     </r>
     <r>
       <rPr>
@@ -2248,34 +2080,57 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
@@ -2452,6 +2307,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2468,7 +2330,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2507,13 +2369,30 @@
   </si>
   <si>
     <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2589,6 +2468,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2625,100 +2510,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2812,6 +2609,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2828,6 +2631,66 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2870,8 +2733,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -2927,33 +2790,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2973,6 +2820,30 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -2981,7 +2852,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2995,7 +2881,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3003,7 +2889,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3019,29 +2919,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3049,22 +2927,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3122,13 +2985,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3146,7 +3003,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3158,13 +3027,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3176,13 +3135,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3200,109 +3159,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3332,16 +3195,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3365,31 +3237,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3415,16 +3278,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3433,148 +3296,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3633,14 +3496,14 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4477,7 +4340,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -4548,7 +4411,7 @@
       <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2"/>
@@ -4575,7 +4438,7 @@
       <c r="F5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="13" t="s">
@@ -4883,25 +4746,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="16" t="s">
+      <c r="G27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>29</v>
-      </c>
       <c r="H27" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4919,7 +4782,7 @@
         <v>22</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4963,13 +4826,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5015,8 +4878,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5091,25 +4954,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="H5" s="13" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5207,22 +5070,22 @@
         <v>3</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>39</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>20</v>
@@ -5312,20 +5175,20 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>20</v>
@@ -5339,7 +5202,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5413,19 +5276,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="E27" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>20</v>
@@ -5442,16 +5305,16 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5489,8 +5352,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5565,25 +5428,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5603,23 +5466,23 @@
         <v>8</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>47</v>
-      </c>
       <c r="D7" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5687,19 +5550,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>20</v>
@@ -5713,20 +5576,20 @@
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -5804,16 +5667,16 @@
         <v>51</v>
       </c>
       <c r="E20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="H20" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5821,21 +5684,21 @@
         <v>8</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5903,25 +5766,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5930,7 +5793,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="15" t="s">
@@ -5981,10 +5844,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>4</v>
@@ -5996,7 +5859,7 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>10</v>
@@ -6037,8 +5900,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6113,25 +5976,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6159,7 +6022,7 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6227,25 +6090,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6256,10 +6119,14 @@
       <c r="C14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6327,10 +6194,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Mon Apr 18 21:48:48 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -1905,7 +1905,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -1939,18 +1939,21 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1991,49 +1994,39 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
     </r>
     <r>
       <rPr>
@@ -2044,97 +2037,62 @@
       </rPr>
       <t xml:space="preserve">
 1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
     </r>
   </si>
   <si>
     <t>跑步45分钟</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2675,6 +2633,60 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>10</t>
     </r>
     <r>
@@ -3441,7 +3453,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3497,9 +3509,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4340,7 +4349,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -4411,7 +4420,7 @@
       <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2"/>
@@ -4878,8 +4887,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5181,14 +5190,14 @@
       <c r="C20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>20</v>
@@ -5276,19 +5285,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="C27" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="D27" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>20</v>
@@ -5305,16 +5314,16 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5428,19 +5437,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>20</v>
@@ -5466,23 +5475,23 @@
         <v>8</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>46</v>
-      </c>
       <c r="D7" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5550,19 +5559,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>20</v>
@@ -5576,20 +5585,20 @@
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -5658,25 +5667,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="D20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="H20" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5684,21 +5693,21 @@
         <v>8</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5766,25 +5775,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5793,7 +5802,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="15" t="s">
@@ -5844,10 +5853,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>4</v>
@@ -5859,7 +5868,7 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>10</v>
@@ -5900,8 +5909,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5976,25 +5985,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6022,7 +6031,7 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6090,25 +6099,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6120,12 +6129,12 @@
         <v>22</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -6194,13 +6203,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>14</v>
@@ -6220,8 +6229,12 @@
         <v>8</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>

</xml_diff>

<commit_message>
Wed May  4 15:13:21 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780" activeTab="2"/>
+    <workbookView windowHeight="16780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="02" sheetId="3" r:id="rId3"/>
     <sheet name="03" sheetId="4" r:id="rId4"/>
     <sheet name="04" sheetId="5" r:id="rId5"/>
+    <sheet name="05" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
   <si>
     <t>早餐</t>
   </si>
@@ -201,15 +202,6 @@
     </r>
   </si>
   <si>
-    <t>背</t>
-  </si>
-  <si>
-    <t>臂</t>
-  </si>
-  <si>
-    <t>肩</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -442,13 +434,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -479,8 +464,37 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
-作业</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
     </r>
   </si>
   <si>
@@ -490,66 +504,7 @@
     <t>胸</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
+    <t>臂</t>
   </si>
   <si>
     <r>
@@ -560,17 +515,7 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
+      <t>10技术书</t>
     </r>
     <r>
       <rPr>
@@ -629,9 +574,74 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>10技术书
 20非技术书</t>
     </r>
@@ -643,74 +653,46 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
-作业</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
+    <t>背</t>
   </si>
   <si>
+    <t>肩</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <strike/>
@@ -733,6 +715,69 @@
     </r>
     <r>
       <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
@@ -860,6 +905,92 @@
         <charset val="134"/>
       </rPr>
       <t>页</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+作业
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
     </r>
   </si>
   <si>
@@ -1722,13 +1853,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1788,6 +1912,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1824,6 +1955,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -1889,17 +2027,14 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
     </r>
     <r>
       <rPr>
@@ -1950,93 +2085,6 @@
         <charset val="134"/>
       </rPr>
       <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
     </r>
   </si>
   <si>
@@ -2048,10 +2096,20 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
     </r>
     <r>
       <rPr>
@@ -2091,18 +2149,51 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2157,6 +2248,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2166,6 +2258,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2175,6 +2268,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2184,12 +2278,49 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
         <charset val="134"/>
       </rPr>
       <t>视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
@@ -2260,18 +2391,21 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
@@ -2288,7 +2422,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2322,35 +2456,28 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2384,40 +2511,17 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
     </r>
   </si>
   <si>
@@ -2471,6 +2575,116 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
@@ -2687,25 +2901,7 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">10技术书
 </t>
     </r>
     <r>
@@ -2733,6 +2929,73 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书
+20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2745,10 +3008,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2791,6 +3054,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <strike/>
@@ -2798,19 +3062,25 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2818,30 +3088,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2856,54 +3102,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2914,16 +3116,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2939,7 +3165,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2979,13 +3242,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="6" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.5"/>
+        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2997,127 +3260,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3135,7 +3290,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3147,13 +3332,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3171,13 +3374,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3206,6 +3469,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3230,17 +3508,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3277,179 +3566,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3475,16 +3738,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3496,19 +3756,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3835,8 +4098,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C10" sqref="$A1:$XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3925,10 +4188,10 @@
       <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3941,8 +4204,8 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4035,10 +4298,10 @@
       <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4048,16 +4311,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4128,21 +4385,21 @@
         <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4166,19 +4423,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -4237,10 +4494,10 @@
       <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4258,13 +4515,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>31</v>
       </c>
     </row>
@@ -4315,28 +4572,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
       <c r="A41" s="9"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
+      <c r="B42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4349,8 +4606,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4402,10 +4659,10 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4417,11 +4674,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4432,26 +4689,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>20</v>
+      <c r="D5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4463,24 +4720,24 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="7" t="s">
-        <v>21</v>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
+      <c r="E7" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
+      <c r="G7" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -4548,26 +4805,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4576,15 +4833,15 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="7" t="s">
-        <v>10</v>
+      <c r="D14" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>12</v>
+      <c r="F14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -4653,7 +4910,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>26</v>
@@ -4662,29 +4919,29 @@
         <v>26</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>22</v>
+      <c r="B21" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="7" t="s">
-        <v>21</v>
+      <c r="E21" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4698,19 +4955,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -4755,25 +5012,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>28</v>
+      <c r="H27" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4781,28 +5038,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="7" t="s">
-        <v>10</v>
+      <c r="C28" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>29</v>
+      <c r="G28" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>31</v>
       </c>
     </row>
@@ -4841,7 +5098,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4853,28 +5110,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
       <c r="A41" s="9"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
+      <c r="B42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4887,8 +5144,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4962,26 +5219,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>31</v>
+      <c r="B5" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>20</v>
+      <c r="G5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4993,24 +5250,24 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>21</v>
+      <c r="C7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
+      <c r="G7" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -5079,44 +5336,44 @@
         <v>3</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>12</v>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="7" t="s">
-        <v>10</v>
+      <c r="D14" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>22</v>
+      <c r="F14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -5185,33 +5442,33 @@
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="H20" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>29</v>
+      <c r="B21" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5228,19 +5485,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -5284,26 +5541,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="C27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="D27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>20</v>
+      <c r="F27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5313,42 +5570,42 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>41</v>
+      <c r="E28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A31" s="10"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="9"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
+      <c r="B32" s="8"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="8"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
+      <c r="B34" s="8"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
       <c r="A35" s="9"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="10"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
+      <c r="B36" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5361,8 +5618,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5436,26 +5693,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>20</v>
+      <c r="H5" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5467,30 +5724,30 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>41</v>
+      <c r="D7" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="F7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5558,47 +5815,47 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>41</v>
+      <c r="B14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>41</v>
+      <c r="F14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -5666,48 +5923,48 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="D20" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="F20" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="G20" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>41</v>
+      <c r="B21" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="15" t="s">
-        <v>41</v>
+      <c r="E21" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>41</v>
+      <c r="G21" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5718,19 +5975,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -5774,26 +6031,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5801,12 +6058,12 @@
         <v>8</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="15" t="s">
-        <v>41</v>
+      <c r="C28" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="15" t="s">
-        <v>22</v>
+      <c r="E28" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -5814,13 +6071,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>31</v>
       </c>
     </row>
@@ -5852,11 +6109,11 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>4</v>
@@ -5867,36 +6124,36 @@
         <v>8</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>10</v>
+      <c r="C35" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
       <c r="A41" s="9"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
+      <c r="B42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5909,8 +6166,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5984,26 +6241,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
+      <c r="B5" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="H5" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6015,8 +6272,8 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -6026,12 +6283,12 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="7" t="s">
-        <v>12</v>
+      <c r="F7" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="7" t="s">
-        <v>55</v>
+      <c r="H7" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6099,25 +6356,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6125,16 +6382,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>55</v>
+      <c r="C14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="7" t="s">
-        <v>55</v>
+      <c r="G14" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -6203,24 +6460,24 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6229,15 +6486,19 @@
         <v>8</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>55</v>
+      <c r="C21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="H21" s="2"/>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6248,19 +6509,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>28</v>
       </c>
     </row>
@@ -6305,24 +6566,24 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6340,10 +6601,10 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>30</v>
       </c>
       <c r="D30" s="9"/>
@@ -6354,7 +6615,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -6362,7 +6623,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="10"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A33" s="4" t="s">
@@ -6370,7 +6631,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
       <c r="A34" s="4" t="s">
@@ -6382,39 +6643,549 @@
       <c r="C34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="B35" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>25</v>
+      </c>
+      <c r="F23" s="7">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
+        <v>30</v>
+      </c>
+      <c r="D30" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="9"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
       <c r="A41" s="9"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
+      <c r="B42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Thu May  5 19:20:53 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780" activeTab="1"/>
+    <workbookView windowHeight="16780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
   <si>
     <t>早餐</t>
   </si>
@@ -994,80 +994,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>校对译稿10页</t>
-    </r>
-  </si>
-  <si>
     <t>腹</t>
   </si>
   <si>
@@ -1883,7 +1809,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 作业
 </t>
     </r>
@@ -2085,6 +2030,42 @@
         <charset val="134"/>
       </rPr>
       <t>1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
@@ -2285,42 +2266,6 @@
         <charset val="134"/>
       </rPr>
       <t>视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
     </r>
   </si>
   <si>
@@ -2530,13 +2475,16 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -2637,16 +2585,13 @@
   </si>
   <si>
     <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
 </t>
     </r>
     <r>
@@ -2674,6 +2619,31 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2960,31 +2930,6 @@
       <t xml:space="preserve">
 1音频/视频
 作业</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
     </r>
   </si>
   <si>
@@ -4606,8 +4551,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5030,7 +4975,7 @@
         <v>28</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5048,7 +4993,7 @@
         <v>19</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5098,7 +5043,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5144,8 +5089,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5220,25 +5165,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5351,10 +5296,10 @@
         <v>22</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5445,22 +5390,22 @@
         <v>22</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5468,7 +5413,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5542,25 +5487,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>37</v>
-      </c>
       <c r="H27" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5618,8 +5563,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5694,10 +5639,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>41</v>
@@ -5709,10 +5654,10 @@
         <v>42</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5732,10 +5677,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>45</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>40</v>
@@ -5745,10 +5690,10 @@
         <v>40</v>
       </c>
       <c r="G7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5816,25 +5761,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5924,25 +5869,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="D20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="F20" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="G20" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5961,7 +5906,7 @@
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>40</v>
@@ -6032,25 +5977,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="F27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6110,13 +6055,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -6166,8 +6111,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6242,10 +6187,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>56</v>
@@ -6257,10 +6202,10 @@
         <v>56</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6371,10 +6316,10 @@
         <v>58</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6566,19 +6511,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="E27" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>63</v>
-      </c>
       <c r="F27" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Fri May 13 18:06:58 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780" activeTab="2"/>
+    <workbookView windowHeight="16780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
   <si>
     <t>早餐</t>
   </si>
@@ -433,71 +433,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>作业</t>
-    </r>
-  </si>
-  <si>
     <t>腿</t>
   </si>
   <si>
@@ -642,6 +577,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书
 20非技术书</t>
     </r>
@@ -909,6 +851,125 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>校对译稿10页</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1779,6 +1840,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -1829,7 +1897,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-作业
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1850,8 +1937,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-二次校对译稿10页
-二次校对译稿10页
 </t>
     </r>
   </si>
@@ -1894,7 +1979,26 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/视频
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 作业</t>
     </r>
   </si>
@@ -2030,42 +2134,6 @@
         <charset val="134"/>
       </rPr>
       <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
     </r>
   </si>
   <si>
@@ -2175,97 +2243,67 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音频</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>视频</t>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
     </r>
   </si>
   <si>
@@ -2285,191 +2323,6 @@
 背</t>
   </si>
   <si>
-    <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/视频</t>
-    </r>
-  </si>
-  <si>
     <t>肩
 跑步45分钟</t>
   </si>
@@ -2492,52 +2345,82 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+作业</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
     </r>
     <r>
       <rPr>
@@ -2566,6 +2449,296 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
@@ -2585,57 +2758,24 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>20非技术书</t>
@@ -2644,106 +2784,12 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>视频</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
@@ -2751,16 +2797,11 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
       <t>10</t>
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2832,7 +2873,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2871,6 +2912,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2879,63 +2926,193 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频
+作业</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/视频
-作业</t>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书
 20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/视频</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
     </r>
     <r>
       <rPr>
@@ -2953,9 +3130,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -2999,7 +3176,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <strike/>
@@ -3007,10 +3183,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3018,6 +3196,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3031,53 +3216,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3092,17 +3232,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3117,17 +3248,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3147,7 +3278,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3205,13 +3382,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3223,55 +3406,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3289,7 +3430,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3301,37 +3508,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3343,49 +3556,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3414,6 +3591,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3429,17 +3621,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3448,7 +3634,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3464,26 +3650,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3511,157 +3677,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3698,25 +3875,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4551,8 +4731,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="E22" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4619,10 +4799,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2"/>
@@ -4634,26 +4814,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>17</v>
+      <c r="H5" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4673,16 +4853,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="13" t="s">
-        <v>20</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -4750,26 +4930,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4778,15 +4958,15 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -4854,39 +5034,39 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>17</v>
+      <c r="B20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>19</v>
+      <c r="B21" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="13" t="s">
-        <v>18</v>
+      <c r="E21" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4956,25 +5136,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="16" t="s">
+      <c r="B27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4983,16 +5163,16 @@
         <v>8</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="13" t="s">
-        <v>24</v>
+      <c r="C28" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="13" t="s">
+      <c r="G28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="12" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5036,13 +5216,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="B34" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -5089,8 +5269,8 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5164,25 +5344,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5203,16 +5383,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>18</v>
+      <c r="C7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="13" t="s">
-        <v>19</v>
+      <c r="G7" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -5280,25 +5460,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5306,19 +5486,19 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>25</v>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="13" t="s">
-        <v>24</v>
+      <c r="D14" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -5386,25 +5566,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="15" t="s">
+      <c r="E20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5412,7 +5592,7 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="2"/>
@@ -5486,25 +5666,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="12" t="s">
+      <c r="G27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5515,17 +5695,17 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>40</v>
+      <c r="E28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5563,8 +5743,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5638,26 +5818,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5676,24 +5856,24 @@
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5760,25 +5940,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5786,21 +5966,21 @@
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>40</v>
+      <c r="B14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>40</v>
+      <c r="F14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -5868,48 +6048,48 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>39</v>
+      <c r="B20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>40</v>
+      <c r="B21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="17" t="s">
-        <v>40</v>
+      <c r="E21" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>40</v>
+      <c r="G21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5976,26 +6156,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>53</v>
+      <c r="B27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6003,12 +6183,12 @@
         <v>8</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="17" t="s">
-        <v>40</v>
+      <c r="C28" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="17" t="s">
-        <v>19</v>
+      <c r="E28" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -6054,14 +6234,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>54</v>
+      <c r="B34" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -6069,11 +6249,11 @@
         <v>8</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>24</v>
+      <c r="C35" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -6111,8 +6291,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6186,26 +6366,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>53</v>
+      <c r="H5" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6228,12 +6408,12 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13" t="s">
-        <v>25</v>
+      <c r="F7" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="13" t="s">
-        <v>57</v>
+      <c r="H7" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6300,26 +6480,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="H13" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6327,16 +6507,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>57</v>
+      <c r="C14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="13" t="s">
-        <v>57</v>
+      <c r="G14" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -6405,7 +6585,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>59</v>
@@ -6420,10 +6600,10 @@
         <v>60</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6431,18 +6611,18 @@
         <v>8</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>57</v>
+      <c r="C21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>57</v>
+      <c r="F21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -6511,25 +6691,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6583,10 +6763,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -6594,8 +6774,8 @@
       <c r="A35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>57</v>
+      <c r="B35" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="8"/>
@@ -6635,8 +6815,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6711,10 +6891,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -6751,8 +6931,12 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>

</xml_diff>

<commit_message>
Tue Aug  9 17:15:56 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="5"/>
+    <workbookView windowHeight="16780" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="05" sheetId="6" r:id="rId6"/>
     <sheet name="06" sheetId="7" r:id="rId7"/>
     <sheet name="07" sheetId="8" r:id="rId8"/>
+    <sheet name="08" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
   <si>
     <t>早餐</t>
   </si>
@@ -37,13 +38,7 @@
   <si>
     <t>10技术书
 20非技术书
-1音频/1视频/10技术书</t>
-  </si>
-  <si>
-    <t>10技术书
-20非技术书
-1音频/1视频/10技术书
-作业</t>
+1音频/1视频/10技术书/1习题</t>
   </si>
   <si>
     <t>问题</t>
@@ -2291,13 +2286,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -2315,41 +2303,64 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -2370,19 +2381,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/1视频/10技术书
-作业</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">10技术书
 </t>
     </r>
     <r>
@@ -2390,20 +2388,30 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作业</t>
     </r>
   </si>
   <si>
@@ -2411,28 +2419,43 @@
   </si>
   <si>
     <r>
-      <rPr>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
         <charset val="134"/>
       </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2443,79 +2466,104 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书</t>
     </r>
   </si>
   <si>
     <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">10技术书
 </t>
     </r>
@@ -2537,8 +2585,7 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/1视频/10技术书
-作业</t>
+1音频/1视频/10技术书/1习题</t>
     </r>
   </si>
   <si>
@@ -2647,97 +2694,27 @@
       </rPr>
       <t>技术书</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>习题</t>
+    </r>
   </si>
   <si>
-    <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>技术书</t>
-    </r>
-  </si>
-  <si>
-    <t>胸
+    <t>腹部，手臂
 慢跑</t>
   </si>
 </sst>
@@ -2746,10 +2723,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2783,6 +2760,13 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2795,16 +2779,70 @@
       <charset val="134"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2818,9 +2856,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2834,22 +2886,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2870,43 +2907,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -2915,44 +2915,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
       <charset val="134"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
@@ -2998,7 +2975,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3010,19 +3023,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3034,85 +3143,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3124,61 +3155,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3207,11 +3184,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3231,17 +3214,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3249,33 +3228,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -3299,8 +3252,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3309,142 +3286,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3454,7 +3431,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3500,13 +3477,16 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3837,7 +3817,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="C10" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3927,15 +3907,15 @@
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3947,7 +3927,7 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -4037,15 +4017,15 @@
         <v>4</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4135,15 +4115,15 @@
         <v>4</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4233,15 +4213,15 @@
         <v>4</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4303,7 +4283,7 @@
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4344,7 +4324,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -4397,10 +4377,10 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4413,10 +4393,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4427,31 +4407,31 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="F5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4463,19 +4443,19 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -4543,43 +4523,43 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -4647,39 +4627,39 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>13</v>
+      <c r="B20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4749,44 +4729,44 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="B27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4829,19 +4809,19 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>27</v>
+      <c r="B34" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4882,7 +4862,7 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="D9" workbookViewId="0">
+    <sheetView topLeftCell="D20" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -4957,31 +4937,31 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>13</v>
+      <c r="H5" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4993,19 +4973,19 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -5073,45 +5053,45 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>33</v>
+      <c r="B13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>15</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -5179,34 +5159,34 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>33</v>
+      <c r="G20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5279,46 +5259,46 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>33</v>
+      <c r="B27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5356,7 +5336,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -5431,31 +5411,31 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>13</v>
+      <c r="B5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -5467,26 +5447,26 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5553,47 +5533,47 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>13</v>
+      <c r="B13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -5661,48 +5641,48 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>13</v>
+      <c r="G20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5769,39 +5749,39 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>33</v>
+      <c r="B27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -5847,26 +5827,26 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>35</v>
+      <c r="B34" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -5904,8 +5884,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5979,31 +5959,31 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -6015,18 +5995,18 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6093,43 +6073,43 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="H13" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -6197,45 +6177,45 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="H20" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -6303,31 +6283,31 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="H27" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -6375,20 +6355,20 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>43</v>
+      <c r="B34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="8"/>
@@ -6428,8 +6408,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6503,31 +6483,31 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -6539,16 +6519,16 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -6617,31 +6597,31 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="H13" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -6650,7 +6630,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6717,31 +6697,31 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6750,7 +6730,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6817,42 +6797,42 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="H27" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -6875,7 +6855,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -6899,26 +6879,26 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="C35" s="19"/>
       <c r="D35" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -6956,8 +6936,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7031,23 +7011,23 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>53</v>
@@ -7055,7 +7035,7 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -7067,7 +7047,7 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="13" t="s">
@@ -7146,19 +7126,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>53</v>
@@ -7169,19 +7149,19 @@
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -7256,34 +7236,34 @@
         <v>56</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -7351,31 +7331,31 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>5</v>
+      <c r="B27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -7384,7 +7364,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7439,10 +7419,12 @@
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="15"/>
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -7480,8 +7462,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7571,15 +7553,15 @@
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -7591,9 +7573,11 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -7681,15 +7665,15 @@
         <v>4</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -7779,15 +7763,15 @@
         <v>4</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -7877,28 +7861,22 @@
         <v>4</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7953,7 +7931,519 @@
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>25</v>
+      </c>
+      <c r="F23" s="7">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
+        <v>30</v>
+      </c>
+      <c r="D30" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>

</xml_diff>

<commit_message>
Mon Aug 29 08:30:43 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16780" activeTab="6"/>
+    <workbookView windowHeight="23980" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="06" sheetId="7" r:id="rId7"/>
     <sheet name="07" sheetId="8" r:id="rId8"/>
     <sheet name="08" sheetId="9" r:id="rId9"/>
+    <sheet name="09" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>早餐</t>
   </si>
@@ -2286,71 +2287,13 @@
   </si>
   <si>
     <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/1视频/10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>作业</t>
-    </r>
-  </si>
-  <si>
-    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -2419,6 +2362,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>10技术书</t>
     </r>
     <r>
@@ -2469,123 +2419,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>1音频/1视频/10技术书</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10技术书
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
     </r>
   </si>
   <si>
@@ -2598,10 +2432,18 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>10</t>
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2647,10 +2489,21 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1</t>
-    </r>
-    <r>
-      <rPr>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2660,6 +2513,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2669,6 +2523,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2678,6 +2533,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2687,6 +2543,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2696,6 +2553,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2705,6 +2563,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2716,6 +2575,90 @@
   <si>
     <t>腹部，手臂
 慢跑</t>
+  </si>
+  <si>
+    <r>
+      <t>10技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <t>跑步</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10技术书
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <t>二头/腹</t>
+  </si>
+  <si>
+    <t>肩膀</t>
   </si>
 </sst>
 </file>
@@ -2723,12 +2666,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2760,7 +2703,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2775,13 +2718,110 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2796,53 +2836,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2856,65 +2850,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -2923,13 +2858,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体-简"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体-简"/>
@@ -2975,13 +2912,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2993,13 +2930,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3017,19 +2996,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3041,31 +3038,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3077,85 +3092,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3184,80 +3121,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -3281,147 +3144,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3431,7 +3368,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3468,29 +3405,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3817,7 +3757,515 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="C7" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>25</v>
+      </c>
+      <c r="F23" s="7">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
+        <v>30</v>
+      </c>
+      <c r="D30" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4392,10 +4840,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2"/>
@@ -4407,25 +4855,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4446,15 +4894,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="2"/>
@@ -4523,25 +4971,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4551,14 +4999,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="2"/>
@@ -4627,25 +5075,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4653,12 +5101,12 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="2"/>
@@ -4729,25 +5177,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4756,16 +5204,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4809,13 +5257,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4937,25 +5385,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4976,15 +5424,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2"/>
@@ -5053,25 +5501,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5079,18 +5527,18 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="2"/>
@@ -5159,25 +5607,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5185,7 +5633,7 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2"/>
@@ -5259,25 +5707,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5288,16 +5736,16 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="14" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5411,25 +5859,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5449,23 +5897,23 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5533,25 +5981,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5559,20 +6007,20 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="15" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="5"/>
@@ -5641,25 +6089,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5667,21 +6115,21 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5749,25 +6197,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5776,11 +6224,11 @@
         <v>6</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="5"/>
@@ -5827,13 +6275,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5842,10 +6290,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5959,25 +6407,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6001,11 +6449,11 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6073,25 +6521,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6100,15 +6548,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -6177,25 +6625,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6204,17 +6652,17 @@
         <v>6</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H21" s="2"/>
@@ -6283,25 +6731,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6355,10 +6803,10 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="10"/>
@@ -6367,7 +6815,7 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="2"/>
@@ -6408,7 +6856,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -6483,25 +6931,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6524,10 +6972,10 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="2"/>
@@ -6597,25 +7045,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6629,7 +7077,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6697,26 +7145,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>47</v>
+      <c r="H20" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6729,7 +7177,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6797,41 +7245,41 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>48</v>
+      <c r="G27" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G28" s="2"/>
@@ -6854,8 +7302,8 @@
         <v>0</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="12" t="s">
-        <v>49</v>
+      <c r="C31" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -6879,25 +7327,25 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>50</v>
+      <c r="B34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="19"/>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6936,8 +7384,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7011,26 +7459,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>51</v>
+      <c r="B5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7050,13 +7498,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="13" t="s">
-        <v>54</v>
+      <c r="C7" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13" t="s">
-        <v>55</v>
+      <c r="F7" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -7125,26 +7573,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>53</v>
+      <c r="B13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7152,15 +7600,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="15" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -7229,40 +7677,40 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>56</v>
+      <c r="B20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2"/>
@@ -7331,26 +7779,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>56</v>
+      <c r="B27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7363,7 +7811,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -7407,24 +7855,24 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>4</v>
+      <c r="B34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -7462,8 +7910,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7537,26 +7985,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>4</v>
+      <c r="B5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7575,7 +8023,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="2"/>
@@ -7649,26 +8097,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>4</v>
+      <c r="B13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7747,26 +8195,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>4</v>
+      <c r="B20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7845,26 +8293,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>4</v>
+      <c r="B27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7919,14 +8367,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>4</v>
+      <c r="B34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7934,8 +8382,8 @@
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="13" t="s">
-        <v>57</v>
+      <c r="C35" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D35" s="2"/>
     </row>
@@ -7974,8 +8422,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8049,26 +8497,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>4</v>
+      <c r="B5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8092,7 +8540,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="2"/>
@@ -8161,26 +8609,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>4</v>
+      <c r="B13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8193,7 +8641,9 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A16" s="2"/>
@@ -8259,35 +8709,41 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>4</v>
+      <c r="B20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="B21" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -8358,13 +8814,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>4</v>
@@ -8383,13 +8839,19 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>

</xml_diff>

<commit_message>
Fri Nov 11 17:08:00 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" firstSheet="7" activeTab="15"/>
+    <workbookView windowHeight="23980" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
   <si>
     <t>早餐</t>
   </si>
@@ -2666,6 +2666,50 @@
   </si>
   <si>
     <r>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -2683,49 +2727,6 @@
         <charset val="134"/>
       </rPr>
       <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
     </r>
     <r>
       <rPr>
@@ -2742,6 +2743,49 @@
     <t>1音频/1视频/10技术书/1习题
 20非技术书
 1音频/1视频/10技术书/1习题</t>
+  </si>
+  <si>
+    <r>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2962,7 +3006,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2984,6 +3028,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3312,103 +3362,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -3423,7 +3473,7 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3444,10 +3494,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3457,7 +3507,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3497,10 +3547,16 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3521,7 +3577,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3929,13 +3985,13 @@
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="24" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -4033,19 +4089,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="24" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -4131,13 +4187,13 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -4431,25 +4487,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4469,7 +4525,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2"/>
@@ -4477,7 +4533,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4545,25 +4601,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4576,10 +4632,10 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4647,25 +4703,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4678,7 +4734,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="2"/>
@@ -4747,25 +4803,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4773,18 +4829,18 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -4831,13 +4887,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4965,25 +5021,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5003,7 +5059,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5089,25 +5145,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5121,19 +5177,19 @@
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5201,25 +5257,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5227,19 +5283,19 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="15" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>55</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -5313,25 +5369,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5345,10 +5401,10 @@
       <c r="C28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -5401,13 +5457,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5415,10 +5471,10 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="15" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="2"/>
@@ -5458,8 +5514,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5533,25 +5589,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5571,25 +5627,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5657,25 +5713,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5686,17 +5742,17 @@
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
@@ -5769,25 +5825,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5795,7 +5851,7 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -5805,10 +5861,10 @@
         <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>13</v>
@@ -5881,25 +5937,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5907,7 +5963,7 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -5917,10 +5973,10 @@
         <v>59</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>13</v>
@@ -5969,13 +6025,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6028,7 +6084,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -6103,25 +6159,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6213,25 +6269,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6311,25 +6367,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6409,25 +6465,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6483,13 +6539,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -7044,8 +7100,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7131,14 +7187,14 @@
       <c r="E5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>61</v>
+      <c r="F5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7229,26 +7285,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>61</v>
+      <c r="B13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7327,26 +7383,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>61</v>
+      <c r="B20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7425,26 +7481,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>61</v>
+      <c r="B27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7499,13 +7555,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -7552,8 +7608,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7628,25 +7684,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7738,24 +7794,24 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7835,25 +7891,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7934,25 +7990,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8136,25 +8192,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8246,25 +8302,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8344,25 +8400,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8644,25 +8700,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8754,25 +8810,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8852,25 +8908,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9144,10 +9200,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2"/>
@@ -9174,10 +9230,10 @@
       <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9198,15 +9254,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="2"/>
@@ -9278,22 +9334,22 @@
       <c r="B13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -9303,14 +9359,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="2"/>
@@ -9379,25 +9435,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9405,12 +9461,12 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="2"/>
@@ -9481,25 +9537,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="22" t="s">
         <v>24</v>
       </c>
     </row>
@@ -9508,16 +9564,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9561,13 +9617,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -9692,22 +9748,22 @@
       <c r="B5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9728,15 +9784,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2"/>
@@ -9805,25 +9861,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -9831,18 +9887,18 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="2"/>
@@ -9911,25 +9967,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -9937,7 +9993,7 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2"/>
@@ -10011,25 +10067,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10040,16 +10096,16 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10163,25 +10219,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10201,23 +10257,23 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="19" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="19" t="s">
         <v>40</v>
       </c>
     </row>
@@ -10285,25 +10341,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10311,20 +10367,20 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="19" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="6"/>
@@ -10393,25 +10449,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10419,21 +10475,21 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="19" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="19" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10501,25 +10557,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10528,11 +10584,11 @@
         <v>6</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="6"/>
@@ -10579,13 +10635,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -10594,10 +10650,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -10711,25 +10767,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10753,11 +10809,11 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -10825,25 +10881,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10852,15 +10908,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -10929,25 +10985,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10956,17 +11012,17 @@
         <v>6</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H21" s="2"/>
@@ -11035,25 +11091,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11107,10 +11163,10 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="10"/>
@@ -11119,7 +11175,7 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="2"/>
@@ -11241,19 +11297,19 @@
       <c r="C5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11276,10 +11332,10 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="15" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="2"/>
@@ -11349,25 +11405,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11381,7 +11437,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -11449,25 +11505,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11481,7 +11537,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -11549,25 +11605,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -11575,15 +11631,15 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="15" t="s">
         <v>44</v>
       </c>
       <c r="G28" s="2"/>
@@ -11606,7 +11662,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="15" t="s">
         <v>48</v>
       </c>
       <c r="D31" s="2"/>
@@ -11631,13 +11687,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>46</v>
       </c>
     </row>
@@ -11645,11 +11701,11 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="14" t="s">
+      <c r="C35" s="21"/>
+      <c r="D35" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -11763,25 +11819,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -11802,12 +11858,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="19" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>51</v>
       </c>
       <c r="G7" s="2"/>
@@ -11877,25 +11933,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -11904,15 +11960,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="19" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -11981,25 +12037,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12007,14 +12063,14 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2"/>
@@ -12083,25 +12139,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12115,7 +12171,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -12159,13 +12215,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12173,10 +12229,10 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -12289,25 +12345,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12327,7 +12383,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="2"/>
@@ -12401,25 +12457,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12499,25 +12555,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12597,25 +12653,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12671,13 +12727,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12686,7 +12742,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="2"/>
@@ -12801,25 +12857,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12844,7 +12900,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="2"/>
@@ -12913,25 +12969,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12945,7 +13001,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>54</v>
       </c>
     </row>
@@ -13013,25 +13069,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13039,13 +13095,13 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="2"/>
@@ -13117,25 +13173,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13143,17 +13199,17 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="15" t="s">
         <v>56</v>
       </c>
     </row>
@@ -13197,13 +13253,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13212,10 +13268,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="15" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tue Nov 29 13:18:24 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23980" firstSheet="7" activeTab="14"/>
+    <workbookView windowHeight="23980" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -24,14 +24,15 @@
     <sheet name="补充2" sheetId="15" r:id="rId15"/>
     <sheet name="补充3" sheetId="16" r:id="rId16"/>
     <sheet name="补充4" sheetId="17" r:id="rId17"/>
-    <sheet name="补充5" sheetId="18" r:id="rId18"/>
+    <sheet name="补充5" sheetId="19" r:id="rId18"/>
+    <sheet name="补充6" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
   <si>
     <t>早餐</t>
   </si>
@@ -2672,6 +2673,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -2685,7 +2687,7 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20</t>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -2695,7 +2697,67 @@
         <rFont val="宋体-简"/>
         <charset val="134"/>
       </rPr>
-      <t>非技术书</t>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/10</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>习题</t>
     </r>
     <r>
       <rPr>
@@ -2710,11 +2772,205 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <charset val="134"/>
-      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">1音频/1视频/10技术书/1习题
 </t>
     </r>
@@ -2726,7 +2982,66 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>20非技术书</t>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
     </r>
     <r>
       <rPr>
@@ -2743,49 +3058,6 @@
     <t>1音频/1视频/10技术书/1习题
 20非技术书
 1音频/1视频/10技术书/1习题</t>
-  </si>
-  <si>
-    <r>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -2793,10 +3065,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2857,38 +3129,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2902,8 +3152,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2918,85 +3259,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体-简"/>
-      <charset val="134"/>
     </font>
     <font>
       <strike/>
@@ -3005,8 +3271,14 @@
       <name val="宋体-简"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体-简"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3039,13 +3311,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3057,31 +3329,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3099,7 +3359,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3117,7 +3389,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3129,7 +3419,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3141,97 +3485,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3284,6 +3550,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3295,15 +3572,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3340,11 +3608,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3362,142 +3628,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3507,7 +3773,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3523,7 +3789,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3541,25 +3807,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3577,7 +3837,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3985,19 +4245,19 @@
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4010,8 +4270,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4089,25 +4349,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4187,13 +4447,13 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -4202,10 +4462,10 @@
       <c r="F20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4300,10 +4560,10 @@
       <c r="F27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4487,25 +4747,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4518,8 +4778,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4601,25 +4861,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4703,25 +4963,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4803,25 +5063,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4887,13 +5147,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4946,8 +5206,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:H7"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5021,25 +5281,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5052,8 +5312,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -5145,25 +5405,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5257,25 +5517,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5369,25 +5629,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5457,13 +5717,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5514,8 +5774,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5589,25 +5849,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5620,8 +5880,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -5713,25 +5973,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5742,22 +6002,22 @@
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5825,25 +6085,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5851,25 +6111,25 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5937,25 +6197,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5963,25 +6223,25 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6025,13 +6285,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6040,13 +6300,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -6084,8 +6344,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6159,25 +6419,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6190,17 +6450,25 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -6269,25 +6537,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6367,25 +6635,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6465,25 +6733,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6539,13 +6807,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6698,8 +6966,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7100,8 +7368,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7206,8 +7474,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7555,14 +7823,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>61</v>
+      <c r="B34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7608,7 +7876,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -7683,26 +7951,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>62</v>
+      <c r="B5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7714,8 +7982,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7793,26 +8061,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>62</v>
+      <c r="B13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7891,26 +8159,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>62</v>
+      <c r="B20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7989,26 +8257,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>62</v>
+      <c r="B27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8063,14 +8331,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>63</v>
+      <c r="B34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -8116,8 +8384,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8191,26 +8459,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>64</v>
+      <c r="B5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8222,8 +8490,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -8301,26 +8569,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>64</v>
+      <c r="B13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8399,26 +8667,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>64</v>
+      <c r="B20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8497,26 +8765,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>63</v>
+      <c r="B27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8571,14 +8839,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>63</v>
+      <c r="B34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -8624,8 +8892,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8699,26 +8967,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>64</v>
+      <c r="B5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8730,8 +8998,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -8809,26 +9077,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>64</v>
+      <c r="B13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8907,26 +9175,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>64</v>
+      <c r="B20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9087,6 +9355,514 @@
       </c>
       <c r="D34" s="6" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="9"/>
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>25</v>
+      </c>
+      <c r="F23" s="7">
+        <v>26</v>
+      </c>
+      <c r="G23" s="7">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="7">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
+        <v>30</v>
+      </c>
+      <c r="D30" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -9203,7 +9979,7 @@
       <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2"/>
@@ -9230,10 +10006,10 @@
       <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9246,8 +10022,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -9334,22 +10110,22 @@
       <c r="B13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -9435,25 +10211,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9537,25 +10313,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -9617,13 +10393,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -9748,22 +10524,22 @@
       <c r="B5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9776,8 +10552,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -9861,25 +10637,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -9967,25 +10743,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10067,25 +10843,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10219,25 +10995,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10250,30 +11026,30 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -10341,25 +11117,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10380,7 +11156,7 @@
       <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="17" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="6"/>
@@ -10449,25 +11225,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10475,21 +11251,21 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="17" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -10557,25 +11333,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10584,11 +11360,11 @@
         <v>6</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="6"/>
@@ -10635,13 +11411,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -10650,10 +11426,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -10767,25 +11543,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10798,8 +11574,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -10881,25 +11657,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10985,25 +11761,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11091,25 +11867,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11163,10 +11939,10 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="10"/>
@@ -11297,19 +12073,19 @@
       <c r="C5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11322,8 +12098,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -11405,25 +12181,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11505,25 +12281,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11605,25 +12381,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -11687,13 +12463,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -11704,7 +12480,7 @@
       <c r="B35" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="15" t="s">
         <v>44</v>
       </c>
@@ -11819,25 +12595,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -11850,20 +12626,20 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="17" t="s">
         <v>51</v>
       </c>
       <c r="G7" s="2"/>
@@ -11933,25 +12709,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -11960,15 +12736,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="17" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -12037,25 +12813,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12063,14 +12839,14 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="17" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2"/>
@@ -12139,25 +12915,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12215,13 +12991,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12232,7 +13008,7 @@
       <c r="B35" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="20"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -12345,25 +13121,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12376,8 +13152,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -12457,25 +13233,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12555,25 +13331,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12653,25 +13429,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12727,13 +13503,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12742,7 +13518,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="17" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="2"/>
@@ -12857,25 +13633,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12888,8 +13664,8 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -12969,25 +13745,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13069,25 +13845,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13173,25 +13949,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13253,13 +14029,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="16" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wed Nov 30 18:18:56 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23980" firstSheet="8" activeTab="16"/>
+    <workbookView windowWidth="28800" windowHeight="13180" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -2767,7 +2767,17 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
     </r>
   </si>
   <si>
@@ -2786,6 +2796,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2795,6 +2806,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2804,6 +2816,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2813,6 +2826,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2822,6 +2836,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2831,6 +2846,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2840,6 +2856,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2849,6 +2866,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -3807,10 +3825,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5774,8 +5792,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:H28"/>
+    <sheetView topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6299,7 +6317,7 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -6935,25 +6953,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7045,25 +7063,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7143,25 +7161,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7241,25 +7259,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7315,13 +7333,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7443,25 +7461,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7553,25 +7571,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7651,25 +7669,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7749,25 +7767,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7823,13 +7841,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7877,7 +7895,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -7951,25 +7969,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8061,25 +8079,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8159,25 +8177,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8257,25 +8275,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8331,13 +8349,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8384,8 +8402,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8569,26 +8587,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>61</v>
+      <c r="B13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8667,26 +8685,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>61</v>
+      <c r="B20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8765,25 +8783,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="C27" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="D27" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="E27" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -8839,13 +8857,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -8892,7 +8910,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -9400,8 +9418,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -9585,20 +9603,20 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>65</v>
+      <c r="B13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>65</v>
@@ -9991,19 +10009,19 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -10107,7 +10125,7 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -10521,7 +10539,7 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -12067,10 +12085,10 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="16" t="s">

</xml_diff>

<commit_message>
Mon Dec 12 08:04:26 CST 2022
</commit_message>
<xml_diff>
--- a/计划/2022学习计划.xlsx
+++ b/计划/2022学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" firstSheet="8" activeTab="16"/>
+    <workbookView windowHeight="23980" firstSheet="8" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -27,12 +27,12 @@
     <sheet name="补充5" sheetId="19" r:id="rId18"/>
     <sheet name="补充6" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74">
   <si>
     <t>早餐</t>
   </si>
@@ -2604,6 +2604,30 @@
     <t>跑</t>
   </si>
   <si>
+    <t>胡辣汤</t>
+  </si>
+  <si>
+    <t>荞麦面</t>
+  </si>
+  <si>
+    <t>菠菜面</t>
+  </si>
+  <si>
+    <t>麻辣拌</t>
+  </si>
+  <si>
+    <t>玉米/红薯/麦片</t>
+  </si>
+  <si>
+    <t>海鲜</t>
+  </si>
+  <si>
+    <t>杂粮面包</t>
+  </si>
+  <si>
+    <t>体重</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <strike/>
@@ -2667,6 +2691,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>1音频/1视频/10技术书/1习题</t>
     </r>
     <r>
@@ -2796,7 +2827,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2806,7 +2836,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2816,7 +2845,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2826,7 +2854,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2836,7 +2863,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2846,7 +2872,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2856,7 +2881,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2866,7 +2890,6 @@
     </r>
     <r>
       <rPr>
-        <strike/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -2890,6 +2913,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>1音频/1视频/10技术书/1习题</t>
@@ -2989,6 +3013,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1音频/1视频/10技术书/1习题
 </t>
     </r>
@@ -3005,55 +3035,6 @@
     <r>
       <rPr>
         <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体-简"/>
@@ -3083,9 +3064,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
@@ -3114,16 +3095,16 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <strike/>
@@ -3148,7 +3129,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3163,47 +3181,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3217,13 +3196,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3234,6 +3207,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3253,14 +3233,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -3268,18 +3240,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3335,7 +3316,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3347,37 +3346,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3389,7 +3358,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3407,25 +3382,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3437,19 +3400,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3461,7 +3436,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3473,19 +3478,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3497,25 +3490,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3544,6 +3525,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3555,26 +3545,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3594,17 +3564,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3627,17 +3602,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3646,142 +3627,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3791,7 +3772,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3825,20 +3806,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3851,12 +3841,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4263,13 +4247,13 @@
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -4367,19 +4351,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="23" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -4465,13 +4449,13 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -4765,25 +4749,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4803,7 +4787,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2"/>
@@ -4811,7 +4795,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4879,25 +4863,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4910,10 +4894,10 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4981,25 +4965,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5012,7 +4996,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="2"/>
@@ -5081,25 +5065,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5107,18 +5091,18 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -5165,13 +5149,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5337,7 +5321,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5455,19 +5439,19 @@
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5561,19 +5545,19 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>55</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -5679,10 +5663,10 @@
       <c r="C28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -5749,10 +5733,10 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="14" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="2"/>
@@ -5792,8 +5776,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5905,25 +5889,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6017,25 +6001,25 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6129,25 +6113,25 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6241,25 +6225,25 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6271,9 +6255,7 @@
       <c r="C30" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
-        <v>31</v>
-      </c>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A31" s="4" t="s">
@@ -6281,7 +6263,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A32" s="4" t="s">
@@ -6289,7 +6271,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A33" s="4" t="s">
@@ -6297,7 +6279,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
       <c r="A34" s="4" t="s">
@@ -6309,23 +6291,19 @@
       <c r="C34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="D35" s="8"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A37" s="8"/>
@@ -6360,13 +6338,13 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
     <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
@@ -6476,20 +6454,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A9" s="2"/>
@@ -6519,7 +6497,9 @@
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6531,10 +6511,16 @@
       <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -6543,91 +6529,121 @@
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="B12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="15">
+        <v>91.7</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A14" s="4" t="s">
+    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3">
+      <c r="B15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C17" s="3">
         <v>16</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D17" s="3">
         <v>17</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E17" s="3">
         <v>18</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F17" s="3">
         <v>19</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G17" s="3">
         <v>20</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A18" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6639,7 +6655,7 @@
     </row>
     <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A19" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -6649,35 +6665,35 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+    <row r="20" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>49</v>
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6687,57 +6703,85 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
+    <row r="22" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3">
         <v>22</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C25" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D25" s="7">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E25" s="7">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F25" s="7">
         <v>26</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G25" s="7">
         <v>27</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H25" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
     </row>
     <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A26" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -6747,125 +6791,223 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>49</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="7">
+      <c r="B31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="2"/>
+      <c r="B33" s="7">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C33" s="7">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D33" s="7">
         <v>31</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A31" s="4" t="s">
+    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A32" s="4" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A35" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
-      <c r="A34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
-    </row>
-    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
-    </row>
-    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" s="1" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A37" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" s="1" customFormat="1" ht="134" customHeight="1" spans="1:9">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="41" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
       <c r="A42" s="9"/>
       <c r="B42" s="8"/>
+    </row>
+    <row r="43" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A43" s="9"/>
+      <c r="B43" s="8"/>
+    </row>
+    <row r="44" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A44" s="9"/>
+      <c r="B44" s="8"/>
+    </row>
+    <row r="45" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A45" s="9"/>
+      <c r="B45" s="10"/>
+    </row>
+    <row r="46" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -6878,7 +7020,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -6953,26 +7095,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>60</v>
+      <c r="B5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7063,26 +7205,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>60</v>
+      <c r="B13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7161,26 +7303,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>60</v>
+      <c r="B20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7259,26 +7401,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>60</v>
+      <c r="B27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7333,14 +7475,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>60</v>
+      <c r="B34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7461,26 +7603,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>60</v>
+      <c r="B5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -7571,26 +7713,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>60</v>
+      <c r="B13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7669,26 +7811,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>60</v>
+      <c r="B20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7767,26 +7909,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>60</v>
+      <c r="B27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -7841,14 +7983,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>60</v>
+      <c r="B34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -7894,7 +8036,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -7969,26 +8111,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>60</v>
+      <c r="B5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8079,26 +8221,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>60</v>
+      <c r="B13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8177,26 +8319,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>60</v>
+      <c r="B20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8275,26 +8417,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>60</v>
+      <c r="B27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8349,14 +8491,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>60</v>
+      <c r="B34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -8402,8 +8544,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8477,26 +8619,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>61</v>
+      <c r="B5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -8588,25 +8730,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8686,25 +8828,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8784,25 +8926,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -8858,13 +9000,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -8910,8 +9052,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8985,26 +9127,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>63</v>
+      <c r="B5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -9095,26 +9237,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>63</v>
+      <c r="B13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9193,26 +9335,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>63</v>
+      <c r="B20" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9292,25 +9434,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9366,13 +9508,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -9409,6 +9551,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -9418,8 +9561,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -9494,25 +9637,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -9604,25 +9747,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9701,26 +9844,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>65</v>
+      <c r="B20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9799,26 +9942,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>66</v>
+      <c r="B27" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -9874,13 +10017,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -9994,10 +10137,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2"/>
@@ -10009,19 +10152,19 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -10048,15 +10191,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="2"/>
@@ -10125,19 +10268,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -10153,14 +10296,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="2"/>
@@ -10229,19 +10372,19 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="13" t="s">
@@ -10255,12 +10398,12 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="2"/>
@@ -10331,25 +10474,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>22</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -10358,16 +10501,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10411,13 +10554,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="19" t="s">
         <v>26</v>
       </c>
     </row>
@@ -10539,19 +10682,19 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -10578,15 +10721,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2"/>
@@ -10655,25 +10798,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10681,18 +10824,18 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="2"/>
@@ -10761,25 +10904,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10787,7 +10930,7 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2"/>
@@ -10876,10 +11019,10 @@
       <c r="F27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -10890,16 +11033,16 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>35</v>
       </c>
     </row>
@@ -11019,13 +11162,13 @@
       <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -11051,23 +11194,23 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -11135,19 +11278,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -11161,20 +11304,20 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="20" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="6"/>
@@ -11243,13 +11386,13 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E20" s="13" t="s">
@@ -11269,21 +11412,21 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="20" t="s">
         <v>35</v>
       </c>
     </row>
@@ -11369,7 +11512,7 @@
       <c r="G27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -11378,11 +11521,11 @@
         <v>6</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="6"/>
@@ -11444,10 +11587,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -11561,19 +11704,19 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -11603,11 +11746,11 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -11675,19 +11818,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -11702,15 +11845,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -11779,19 +11922,19 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G20" s="13" t="s">
@@ -11806,17 +11949,17 @@
         <v>6</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>44</v>
       </c>
       <c r="H21" s="2"/>
@@ -11885,19 +12028,19 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G27" s="13" t="s">
@@ -11957,10 +12100,10 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="19" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="10"/>
@@ -11969,7 +12112,7 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="2"/>
@@ -12085,19 +12228,19 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -12126,10 +12269,10 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="2"/>
@@ -12199,19 +12342,19 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -12231,7 +12374,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -12331,7 +12474,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -12425,15 +12568,15 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G28" s="2"/>
@@ -12456,7 +12599,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D31" s="2"/>
@@ -12495,11 +12638,11 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="15" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -12652,12 +12795,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="20" t="s">
         <v>51</v>
       </c>
       <c r="G7" s="2"/>
@@ -12730,22 +12873,22 @@
       <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12754,15 +12897,15 @@
         <v>6</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="20" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -12831,25 +12974,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12857,14 +13000,14 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="20" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2"/>
@@ -12933,25 +13076,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -12965,7 +13108,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -13009,13 +13152,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13023,10 +13166,10 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -13139,25 +13282,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13177,7 +13320,7 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="2"/>
@@ -13251,25 +13394,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13349,25 +13492,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13447,25 +13590,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13521,13 +13664,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13536,7 +13679,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="2"/>
@@ -13651,25 +13794,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13694,7 +13837,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="2"/>
@@ -13763,25 +13906,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13795,7 +13938,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>54</v>
       </c>
     </row>
@@ -13863,25 +14006,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13889,13 +14032,13 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="2"/>
@@ -13967,25 +14110,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13993,17 +14136,17 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>56</v>
       </c>
     </row>
@@ -14047,13 +14190,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -14062,10 +14205,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>